<commit_message>
Mise à jour des plan de Test
</commit_message>
<xml_diff>
--- a/Documentation/Test.xlsx
+++ b/Documentation/Test.xlsx
@@ -7,16 +7,19 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan de test" sheetId="1" r:id="rId1"/>
+    <sheet name="Rapport de test complet" sheetId="2" r:id="rId2"/>
+    <sheet name="Rapport de test restreint" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plan de test'!$A:$D</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Action</t>
   </si>
@@ -115,6 +118,219 @@
   </si>
   <si>
     <t>Prérequi</t>
+  </si>
+  <si>
+    <t>L'utilisateur ferme le panneau de navigation à l'aide de la flèche</t>
+  </si>
+  <si>
+    <t>Click sur un tracé</t>
+  </si>
+  <si>
+    <t>Séléction d'un panneau correspondant à un voyage</t>
+  </si>
+  <si>
+    <t>Fermeture d'un panneau correspondant à un voyage</t>
+  </si>
+  <si>
+    <t>Click sur un marqueur correspondant  à une étape</t>
+  </si>
+  <si>
+    <t>Séléction d'une étape dans la liste d'un panneau correspondant à un voyage</t>
+  </si>
+  <si>
+    <t>Ouverture du panneau de navigation à l'aide de la miniature</t>
+  </si>
+  <si>
+    <t>Ouverture du panneau de navigation à l'aide de la miniature lorsque le panneau d'apperçu est ouvert</t>
+  </si>
+  <si>
+    <t>Chargement d'une étape contenant des média</t>
+  </si>
+  <si>
+    <t>Chargement d'une étape ne contenant pas de média</t>
+  </si>
+  <si>
+    <t>Ouverture de l'interface de création à l'aide de la miniature</t>
+  </si>
+  <si>
+    <t>Ajout d'une nouvelle étape à l'aide du bouton</t>
+  </si>
+  <si>
+    <t>Ouverture du panel de l'étape</t>
+  </si>
+  <si>
+    <t>Édition du titre de l'étape</t>
+  </si>
+  <si>
+    <t>Séléction de la date</t>
+  </si>
+  <si>
+    <t>Click du bouton de géolocalisation</t>
+  </si>
+  <si>
+    <t>Click du bouton de recherche lorsque le champ d'adresse est vide</t>
+  </si>
+  <si>
+    <t>Click du bouton de recherche lorsque le champ d'adresse contient une addresse bidon</t>
+  </si>
+  <si>
+    <t>Click du bouton de recherche lorsque le champs d'adresse conteient une addresse valide</t>
+  </si>
+  <si>
+    <t>Fermeture d'un panneau correspondant à une étape</t>
+  </si>
+  <si>
+    <t>Ouverture d'un panneau correspondant à une étape lorsqu'un autre panneau du même genre est ouvert</t>
+  </si>
+  <si>
+    <t>Click sur la map lorsq'un paneau est ouvert</t>
+  </si>
+  <si>
+    <t>Click sur la map lorsqu'aucun paneau est fermé</t>
+  </si>
+  <si>
+    <t>Le marqueur de l'étape précédente est défini. Définition du marqueur de l'étape.</t>
+  </si>
+  <si>
+    <t>Le marqueur de l'étape suivant est défini. Définition du marqueur de l'étape.</t>
+  </si>
+  <si>
+    <t>Le marqueur de l'étape précédente et celle de l'étape suivant est défini. Définition du marqueur de l'étape</t>
+  </si>
+  <si>
+    <t>Trois étapes possèdent des marqueurs défini. On redéfini le marqueur du millieux.</t>
+  </si>
+  <si>
+    <t>Trois étapes possèdent des marqueurs défini. On supprime l'étape du millieux</t>
+  </si>
+  <si>
+    <t>L'étapes d'avant et celle d'après possèdent des marqueus. On supprime l'étape du millieux, qui n'a pas de marqueur.</t>
+  </si>
+  <si>
+    <t>On click sur la croix à côté du titre de l'étape</t>
+  </si>
+  <si>
+    <t>On confirme la suppression</t>
+  </si>
+  <si>
+    <t>On décline la confirmation</t>
+  </si>
+  <si>
+    <t>On tente de quitter l'interface de création</t>
+  </si>
+  <si>
+    <t>On confirme vouloir quitter l'interface de création</t>
+  </si>
+  <si>
+    <t>On décline vouloir quiter l'interface de création</t>
+  </si>
+  <si>
+    <t>On valide un voyage ne contenant qu'une étape</t>
+  </si>
+  <si>
+    <t>ON valide un voyage ne contenant pas de titre</t>
+  </si>
+  <si>
+    <t>On valide un voyage dont les date sont incohérentes</t>
+  </si>
+  <si>
+    <t>ON valide un voyage dont tout les marqueurs ne sont pas définis</t>
+  </si>
+  <si>
+    <t>On valide un voyage dont une des étape ne contient pas de commentaires</t>
+  </si>
+  <si>
+    <t>Deux marqueurs adjacents sont accessible par la terre</t>
+  </si>
+  <si>
+    <t>Deux marqueurs adjacents sont accessible par les aires</t>
+  </si>
+  <si>
+    <t>On click au millieux d'un océan pour définir un marqueur</t>
+  </si>
+  <si>
+    <t>Deux marqueurs adjacents sont accessibles par la terre</t>
+  </si>
+  <si>
+    <t>Deux marqueurs adjacents sont accessibles par les aires</t>
+  </si>
+  <si>
+    <t>On click sur l'icone d'image pour sélectioner des images</t>
+  </si>
+  <si>
+    <t>On sélectionne une image et on valide</t>
+  </si>
+  <si>
+    <t>On sélectionne deux images et on valide</t>
+  </si>
+  <si>
+    <t>ON sélectionne plus de dix images</t>
+  </si>
+  <si>
+    <t>On sélectionne un image dépassant la limite autorisée</t>
+  </si>
+  <si>
+    <t>On suprime toute les images à l'aide de l'icone poubelle</t>
+  </si>
+  <si>
+    <t>On suprime une image à l'aide de son icone poubelle</t>
+  </si>
+  <si>
+    <t>On tente de charger un fichier qui n'est pas une image</t>
+  </si>
+  <si>
+    <t>On tente valide un voyage correcte</t>
+  </si>
+  <si>
+    <t>On tente de supprimer un voyage en clickant sur la croix à côté de son panneau dans la navigation</t>
+  </si>
+  <si>
+    <t>ON valide un voyage ayant pour effet d'ajouter un page</t>
+  </si>
+  <si>
+    <t>On tente de modifier un voyage en clickant sur le crayon à côté de son titre dans la navigation</t>
+  </si>
+  <si>
+    <t>On supprime l'une des étape, puis on valide</t>
+  </si>
+  <si>
+    <t>On ajoute une étape, puis on valide</t>
+  </si>
+  <si>
+    <t>On modifie une étape, puis on valide</t>
+  </si>
+  <si>
+    <t>On modifie l'emplacement du marqueur d'une étape existante</t>
+  </si>
+  <si>
+    <t>On modifie le titre du voyage</t>
+  </si>
+  <si>
+    <t>On supprime une image, puis on valide</t>
+  </si>
+  <si>
+    <t>ON supprime une image, puis on quite l'interface. On ouvre ensuite un autre voyage en modification, on supprime une autre étape, puis on valide</t>
+  </si>
+  <si>
+    <t>On ajoute une image à une étape en contenant déjà</t>
+  </si>
+  <si>
+    <t>On tente de charger plus de dix images au total en comptant les images pré-visualisées dans le cas ou une étape en possède déjà</t>
+  </si>
+  <si>
+    <t>Sur la carte, on tente de dézoomer le plus possible</t>
+  </si>
+  <si>
+    <t>Sur la carte, on tente de dépasser du pôle nord en la déplaçant à l'aide de la souris</t>
+  </si>
+  <si>
+    <t>Sur la carte, on tente de dépasser du pôle sud en la déplaçant à l'aide de la souris</t>
+  </si>
+  <si>
+    <t>Une fois au bord de la carte, au niveau du pôle nord, à un niveau de zoom élevé, on dézoom</t>
+  </si>
+  <si>
+    <t>Une fois au bord de la carte, au niveau du pôle sud à un niveau de zoom élevé, on dézoom</t>
   </si>
 </sst>
 </file>
@@ -477,19 +693,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="94" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,181 +924,569 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C48" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug réglé : le rapport de test est full Positif
</commit_message>
<xml_diff>
--- a/Documentation/Test.xlsx
+++ b/Documentation/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="299">
   <si>
     <t>N°</t>
   </si>
@@ -234,9 +234,6 @@
     <t>On valide un voyage ne contenant qu'une étape</t>
   </si>
   <si>
-    <t>ON valide un voyage ne contenant pas de titre</t>
-  </si>
-  <si>
     <t>On valide un voyage dont les date sont incohérentes</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
   </si>
   <si>
     <t>On supprime une image, puis on valide</t>
-  </si>
-  <si>
-    <t>ON supprime une image, puis on quite l'interface. On ouvre ensuite un autre voyage en modification, on supprime une autre étape, puis on valide</t>
   </si>
   <si>
     <t>On ajoute une image à une étape en contenant déjà</t>
@@ -869,6 +863,69 @@
   </si>
   <si>
     <t>Le voyage est supprimé et la navvigation se rechaarge</t>
+  </si>
+  <si>
+    <t>L'interface de création s'ouvre avec les panneaux des étapes générés et les informations chargées dans les champs</t>
+  </si>
+  <si>
+    <t>Une fois retourné dans la navigation, l'étape apparait à la suite des autres. Le tracé à également été mis à jour.</t>
+  </si>
+  <si>
+    <t>Une fois retourné dans la navigation, l'étape  s'apparait plus. Le tracé à également été mis à jour.</t>
+  </si>
+  <si>
+    <t>Lorsqu'on charge ses détails dans la navigation, on voit qu'elles ont bien été modifiées</t>
+  </si>
+  <si>
+    <t>De retour à la navigation, le marqueur a bien été déplacé ainsi que son tracé a été mis à jour</t>
+  </si>
+  <si>
+    <t>Le titre du panneau appararait dans la navigation tel qu'il a ét modifié</t>
+  </si>
+  <si>
+    <t>Lorsqu'on charge ses détails dans la navigation, on voit que l'image a bien été supprimée.</t>
+  </si>
+  <si>
+    <t>On supprime une image, puis on quite l'interface. On ouvre ensuite un autre voyage en modification, on supprime une autre étape, puis on valide</t>
+  </si>
+  <si>
+    <t>La permière image a persisté alors que la seconde été supprimée</t>
+  </si>
+  <si>
+    <t>Les images existante sont conservées et la nouvelle image est ajoutée à la base</t>
+  </si>
+  <si>
+    <t>Les image issue du serveur sont bien prises en compte et il n'est pas possible de dépasser dix images</t>
+  </si>
+  <si>
+    <t>La map bloque à partir d'un certain point</t>
+  </si>
+  <si>
+    <t>Arrivé à la limite, le déplacement est bloqué dans cette direction</t>
+  </si>
+  <si>
+    <t>Le centre va se décaler vers l'équateur au fur et à mesur que le zoom diminue, de telle sorte à ne pas sortir des limites</t>
+  </si>
+  <si>
+    <t>Lundi 19 Juin 2015</t>
+  </si>
+  <si>
+    <t>Lundi 19 Juin 2016</t>
+  </si>
+  <si>
+    <t>Non Conforme</t>
+  </si>
+  <si>
+    <t>Souvent Conforme</t>
+  </si>
+  <si>
+    <t>Le DatePicker se bloque parfois</t>
+  </si>
+  <si>
+    <t>On valide un voyage ne contenant pas de titre</t>
+  </si>
+  <si>
+    <t>Problème lors du chargement des routes : fait planter l'application</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1023,6 +1080,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1044,26 +1122,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1381,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1429,13 +1489,13 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>182</v>
+      <c r="C3" s="24" t="s">
+        <v>180</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -1446,12 +1506,12 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1461,43 +1521,43 @@
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>183</v>
+      <c r="C7" s="24" t="s">
+        <v>181</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>11</v>
@@ -1508,12 +1568,12 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1523,14 +1583,14 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>14</v>
@@ -1538,14 +1598,14 @@
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>15</v>
@@ -1553,14 +1613,14 @@
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>16</v>
@@ -1568,14 +1628,14 @@
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>17</v>
@@ -1583,12 +1643,12 @@
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1598,17 +1658,17 @@
     </row>
     <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="4">
         <v>3</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -1616,46 +1676,46 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>184</v>
+        <v>192</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>182</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="12">
         <v>6</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="22">
+        <v>115</v>
+      </c>
+      <c r="B17" s="15">
         <v>6</v>
       </c>
-      <c r="C17" s="19"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1665,7 +1725,7 @@
       <c r="B18" s="4">
         <v>7</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1675,42 +1735,42 @@
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="12">
         <v>8</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B20" s="12">
         <v>8</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="12">
         <v>9</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
@@ -1720,12 +1780,12 @@
     </row>
     <row r="22" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B22" s="12">
         <v>9</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1735,12 +1795,12 @@
     </row>
     <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="12">
         <v>9</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="5" t="s">
         <v>30</v>
       </c>
@@ -1750,89 +1810,89 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="12">
         <v>8</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B25" s="12">
         <v>8</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" s="12">
         <v>1</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>185</v>
+      <c r="C26" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B27" s="12">
         <v>8</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="12">
         <v>7</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" s="12">
         <v>13</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="5" t="s">
         <v>39</v>
       </c>
@@ -1842,72 +1902,72 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="15"/>
+        <v>126</v>
+      </c>
+      <c r="C30" s="22"/>
       <c r="D30" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B31" s="12">
         <v>14</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B32" s="12">
         <v>14</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" s="12">
         <v>14</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B34" s="12">
         <v>14</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="5" t="s">
         <v>45</v>
       </c>
@@ -1917,12 +1977,12 @@
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" s="12">
         <v>14</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="5" t="s">
         <v>47</v>
       </c>
@@ -1932,12 +1992,12 @@
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B36" s="12">
         <v>14</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="5" t="s">
         <v>49</v>
       </c>
@@ -1947,12 +2007,12 @@
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="C37" s="15"/>
+        <v>195</v>
+      </c>
+      <c r="C37" s="22"/>
       <c r="D37" s="5" t="s">
         <v>51</v>
       </c>
@@ -1962,12 +2022,12 @@
     </row>
     <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B38" s="12">
         <v>14</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="5" t="s">
         <v>53</v>
       </c>
@@ -1977,12 +2037,12 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B39" s="12">
         <v>14</v>
       </c>
-      <c r="C39" s="15"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="5" t="s">
         <v>55</v>
       </c>
@@ -1992,12 +2052,12 @@
     </row>
     <row r="40" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B40" s="12">
         <v>16</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="5" t="s">
         <v>56</v>
       </c>
@@ -2007,12 +2067,12 @@
     </row>
     <row r="41" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B41" s="12">
         <v>16</v>
       </c>
-      <c r="C41" s="15"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="5" t="s">
         <v>58</v>
       </c>
@@ -2022,27 +2082,27 @@
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B42" s="12">
         <v>16</v>
       </c>
-      <c r="C42" s="15"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B43" s="12">
         <v>16</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="5" t="s">
         <v>60</v>
       </c>
@@ -2050,12 +2110,12 @@
     </row>
     <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44" s="15"/>
+        <v>193</v>
+      </c>
+      <c r="C44" s="22"/>
       <c r="D44" s="5" t="s">
         <v>61</v>
       </c>
@@ -2065,27 +2125,27 @@
     </row>
     <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C45" s="15"/>
+        <v>193</v>
+      </c>
+      <c r="C45" s="22"/>
       <c r="D45" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B46" s="12">
         <v>14</v>
       </c>
-      <c r="C46" s="15"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="5" t="s">
         <v>63</v>
       </c>
@@ -2095,27 +2155,27 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C47" s="15"/>
+        <v>196</v>
+      </c>
+      <c r="C47" s="22"/>
       <c r="D47" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C48" s="15"/>
+        <v>196</v>
+      </c>
+      <c r="C48" s="22"/>
       <c r="D48" s="5" t="s">
         <v>66</v>
       </c>
@@ -2125,42 +2185,42 @@
     </row>
     <row r="49" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B49" s="12">
         <v>13</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="5" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B50" s="12">
         <v>13</v>
       </c>
-      <c r="C50" s="15"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B51" s="12">
         <v>13</v>
       </c>
-      <c r="C51" s="15"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="5" t="s">
         <v>69</v>
       </c>
@@ -2170,257 +2230,257 @@
     </row>
     <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B52" s="12">
         <v>15</v>
       </c>
-      <c r="C52" s="15"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B53" s="12">
         <v>15</v>
       </c>
-      <c r="C53" s="15"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="5" t="s">
-        <v>71</v>
+        <v>297</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B54" s="12">
         <v>15</v>
       </c>
-      <c r="C54" s="15"/>
+      <c r="C54" s="22"/>
       <c r="D54" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B55" s="12">
         <v>16</v>
       </c>
-      <c r="C55" s="15"/>
+      <c r="C55" s="22"/>
       <c r="D55" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B56" s="12">
         <v>15</v>
       </c>
-      <c r="C56" s="15"/>
+      <c r="C56" s="22"/>
       <c r="D56" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B57" s="12">
         <v>17</v>
       </c>
-      <c r="C57" s="15"/>
+      <c r="C57" s="22"/>
       <c r="D57" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B58" s="12">
         <v>17</v>
       </c>
-      <c r="C58" s="15"/>
+      <c r="C58" s="22"/>
       <c r="D58" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C59" s="15"/>
+        <v>194</v>
+      </c>
+      <c r="C59" s="22"/>
       <c r="D59" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B60" s="12">
         <v>14</v>
       </c>
-      <c r="C60" s="15"/>
+      <c r="C60" s="22"/>
       <c r="D60" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B61" s="12">
         <v>14</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" s="22"/>
       <c r="D61" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B62" s="12">
         <v>14</v>
       </c>
-      <c r="C62" s="15"/>
+      <c r="C62" s="22"/>
       <c r="D62" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B63" s="12">
         <v>14</v>
       </c>
-      <c r="C63" s="15"/>
+      <c r="C63" s="22"/>
       <c r="D63" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B64" s="12">
         <v>14</v>
       </c>
-      <c r="C64" s="15"/>
+      <c r="C64" s="22"/>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B65" s="12">
         <v>14</v>
       </c>
-      <c r="C65" s="15"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B66" s="12">
         <v>14</v>
       </c>
-      <c r="C66" s="15"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B67" s="12">
         <v>14</v>
       </c>
-      <c r="C67" s="15"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B68" s="12">
         <v>16</v>
       </c>
-      <c r="C68" s="15"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2430,192 +2490,212 @@
       <c r="B69" s="12">
         <v>16</v>
       </c>
-      <c r="C69" s="16"/>
+      <c r="C69" s="23"/>
       <c r="D69" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B70" s="12">
         <v>6</v>
       </c>
-      <c r="C70" s="14" t="s">
-        <v>186</v>
+      <c r="C70" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C71" s="15"/>
+      <c r="C71" s="22"/>
       <c r="D71" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B72" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="E72" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>23</v>
       </c>
       <c r="B73" s="12">
         <v>6</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>187</v>
+      <c r="C73" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E73" s="11"/>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B74" s="12">
         <v>23</v>
       </c>
-      <c r="C74" s="15"/>
+      <c r="C74" s="22"/>
       <c r="D74" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E74" s="11"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B75" s="12">
         <v>23</v>
       </c>
-      <c r="C75" s="15"/>
+      <c r="C75" s="22"/>
       <c r="D75" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B76" s="12">
         <v>23</v>
       </c>
-      <c r="C76" s="15"/>
+      <c r="C76" s="22"/>
       <c r="D76" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B77" s="12">
         <v>23</v>
       </c>
-      <c r="C77" s="15"/>
+      <c r="C77" s="22"/>
       <c r="D77" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" s="11"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B78" s="12">
         <v>23</v>
       </c>
-      <c r="C78" s="15"/>
+      <c r="C78" s="22"/>
       <c r="D78" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E78" s="11"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B79" s="12">
         <v>23</v>
       </c>
-      <c r="C79" s="15"/>
+      <c r="C79" s="22"/>
       <c r="D79" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E79" s="11"/>
+        <v>92</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B80" s="12">
         <v>23</v>
       </c>
-      <c r="C80" s="15"/>
+      <c r="C80" s="22"/>
       <c r="D80" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E80" s="11"/>
-    </row>
-    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B81" s="12">
         <v>23</v>
       </c>
-      <c r="C81" s="15"/>
+      <c r="C81" s="22"/>
       <c r="D81" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E81" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B82" s="12">
         <v>23</v>
       </c>
-      <c r="C82" s="16"/>
+      <c r="C82" s="23"/>
       <c r="D82" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E82" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
@@ -2624,13 +2704,15 @@
       <c r="B83" s="12">
         <v>6</v>
       </c>
-      <c r="C83" s="14" t="s">
-        <v>188</v>
+      <c r="C83" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E83" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
@@ -2639,50 +2721,58 @@
       <c r="B84" s="12">
         <v>6</v>
       </c>
-      <c r="C84" s="15"/>
+      <c r="C84" s="22"/>
       <c r="D84" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E84" s="11"/>
-    </row>
-    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B85" s="12">
         <v>6</v>
       </c>
-      <c r="C85" s="15"/>
+      <c r="C85" s="22"/>
       <c r="D85" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E85" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B86" s="12">
         <v>6</v>
       </c>
-      <c r="C86" s="15"/>
+      <c r="C86" s="22"/>
       <c r="D86" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E86" s="11"/>
-    </row>
-    <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
-      <c r="C87" s="16"/>
+      <c r="C87" s="23"/>
       <c r="D87" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E87" s="11"/>
+        <v>99</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
@@ -2708,17 +2798,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="16" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2727,13 +2817,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,154 +2831,154 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D14" s="10"/>
     </row>
@@ -2897,34 +2987,34 @@
         <v>6</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D17" s="10"/>
     </row>
@@ -2933,541 +3023,625 @@
         <v>8</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C29" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C31" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C33" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C34" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C35" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C36" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C37" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C38" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C39" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C40" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C41" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C42" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C46" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C50" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C51" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C53" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C54" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C55" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C56" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C57" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C58" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D58" s="10"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C59" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C60" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C61" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C62" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C63" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C64" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C65" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D65" s="10"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C66" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C67" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C68" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C69" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D69" s="10"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,174 +3649,232 @@
         <v>21</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C70" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>22</v>
+      <c r="A71" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C71" s="22"/>
+        <v>292</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>23</v>
+      <c r="A72" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C72" s="22"/>
+        <v>293</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>170</v>
+        <v>272</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C73" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>171</v>
+      <c r="A74" s="4">
+        <v>23</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C74" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C75" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C76" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C77" s="22"/>
-      <c r="D77" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="11"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="11"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="11"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C81" s="22"/>
-      <c r="D81" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" s="11"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C82" s="22"/>
-      <c r="D82" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D82" s="11"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C83" s="22"/>
-      <c r="D83" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D83" s="11"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C84" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D84" s="10"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>179</v>
+        <v>35</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C85" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>180</v>
+        <v>37</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C86" s="22"/>
+        <v>190</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="D86" s="10"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D87" s="10"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D88" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3650,326 +3882,328 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="18" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C11" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
-        <v>5</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>8</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>9</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C12" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>13</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>12</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="C13" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>14</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
-        <v>13</v>
-      </c>
-      <c r="B13" s="21" t="s">
+      <c r="C14" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:4" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
-        <v>14</v>
-      </c>
-      <c r="B14" s="21" t="s">
+      <c r="C15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>16</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
-        <v>15</v>
-      </c>
-      <c r="B15" s="27" t="s">
+      <c r="C16" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>17</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
-        <v>16</v>
-      </c>
-      <c r="B16" s="11" t="s">
+      <c r="C17" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>18</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>17</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="C18" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>19</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>18</v>
-      </c>
-      <c r="B18" s="21" t="s">
+      <c r="C19" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>20</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>19</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="C20" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>21</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
-        <v>20</v>
-      </c>
-      <c r="B20" s="21" t="s">
+      <c r="C21" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>22</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
-        <v>21</v>
-      </c>
-      <c r="B21" s="21" t="s">
+      <c r="C22" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>23</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
-        <v>22</v>
-      </c>
-      <c r="B22" s="21" t="s">
+      <c r="C23" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>24</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>25</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
-        <v>23</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
-        <v>24</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
-        <v>25</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>246</v>
+      <c r="C25" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>